<commit_message>
[add]poi import excel template
</commit_message>
<xml_diff>
--- a/o-pdf-exporter/template/template.xlsx
+++ b/o-pdf-exporter/template/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>站点名称</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>跟进中</t>
+  </si>
+  <si>
+    <t>签名</t>
+  </si>
+  <si>
+    <t>${signName}</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1031,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6428571428571" defaultRowHeight="26" customHeight="1" outlineLevelRow="7" outlineLevelCol="6"/>
@@ -1093,6 +1099,14 @@
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="6:7">
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="3:3">

</xml_diff>